<commit_message>
excel could not done
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/Test.xlsx
+++ b/src/main/java/com/testdata/Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{4812226B-C8F1-4011-9601-0A777C049F4A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{D6D3D6FD-EA26-42FA-9E9D-70C62DA95520}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="5805" xr2:uid="{8FF49A41-D681-4C84-BD33-FF869755A9FC}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Firstname</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>aP1</t>
+  </si>
+  <si>
+    <t>123-1</t>
+  </si>
+  <si>
+    <t>124-2</t>
+  </si>
+  <si>
+    <t>125-3</t>
+  </si>
+  <si>
+    <t>126-4</t>
+  </si>
+  <si>
+    <t>127-5</t>
+  </si>
+  <si>
+    <t>128-6</t>
+  </si>
+  <si>
+    <t>129-7</t>
+  </si>
+  <si>
+    <t>130-8</t>
   </si>
 </sst>
 </file>
@@ -459,7 +483,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,8 +518,8 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
-        <v>123</v>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -508,8 +532,8 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3">
-        <v>124</v>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -522,8 +546,8 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3">
-        <v>125</v>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,8 +560,8 @@
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3">
-        <v>126</v>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -550,8 +574,8 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
-        <v>127</v>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,8 +588,8 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3">
-        <v>128</v>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -578,8 +602,8 @@
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3">
-        <v>129</v>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,8 +616,8 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3">
-        <v>130</v>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
customer class and update credentials test
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/Test.xlsx
+++ b/src/main/java/com/testdata/Test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{D6D3D6FD-EA26-42FA-9E9D-70C62DA95520}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{29F50884-B0C6-437B-B519-84E93D7F6DFD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="5805" xr2:uid="{8FF49A41-D681-4C84-BD33-FF869755A9FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="5895" xr2:uid="{8FF49A41-D681-4C84-BD33-FF869755A9FC}"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Firstname</t>
   </si>
@@ -84,30 +84,6 @@
   </si>
   <si>
     <t>aP1</t>
-  </si>
-  <si>
-    <t>123-1</t>
-  </si>
-  <si>
-    <t>124-2</t>
-  </si>
-  <si>
-    <t>125-3</t>
-  </si>
-  <si>
-    <t>126-4</t>
-  </si>
-  <si>
-    <t>127-5</t>
-  </si>
-  <si>
-    <t>128-6</t>
-  </si>
-  <si>
-    <t>129-7</t>
-  </si>
-  <si>
-    <t>130-8</t>
   </si>
 </sst>
 </file>
@@ -483,7 +459,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,8 +494,8 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
+      <c r="D2" s="3">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -532,8 +508,8 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
+      <c r="D3" s="3">
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -546,8 +522,8 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
+      <c r="D4" s="3">
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -560,8 +536,8 @@
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
+      <c r="D5" s="3">
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,8 +550,8 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
+      <c r="D6" s="3">
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -588,8 +564,8 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
+      <c r="D7" s="3">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -602,8 +578,8 @@
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
+      <c r="D8" s="3">
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,8 +592,8 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
+      <c r="D9" s="3">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Scheduled maint class
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/Test.xlsx
+++ b/src/main/java/com/testdata/Test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{29F50884-B0C6-437B-B519-84E93D7F6DFD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{3ACF4F4D-249B-42AD-9B05-BA497C08A448}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="5895" xr2:uid="{8FF49A41-D681-4C84-BD33-FF869755A9FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="5895" xr2:uid="{8FF49A41-D681-4C84-BD33-FF869755A9FC}"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Firstname</t>
   </si>
@@ -29,9 +29,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>ap1</t>
-  </si>
-  <si>
     <t>ap@g.com</t>
   </si>
   <si>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t>aP1</t>
+  </si>
+  <si>
+    <t>394-357</t>
+  </si>
+  <si>
+    <t>319-86</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,25 +477,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="D2" s="3">
         <v>123</v>
@@ -500,13 +503,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>124</v>
@@ -514,13 +517,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3">
         <v>125</v>
@@ -528,13 +531,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
         <v>126</v>
@@ -542,13 +545,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3">
         <v>127</v>
@@ -556,13 +559,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3">
         <v>128</v>
@@ -570,13 +573,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3">
         <v>129</v>
@@ -584,13 +587,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3">
         <v>130</v>

</xml_diff>

<commit_message>
if there are any
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/Test.xlsx
+++ b/src/main/java/com/testdata/Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{D1712989-89F3-4252-B1EB-99AD06085025}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{503E70A1-B813-4B39-BA1E-24B97DEF27D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16530" windowHeight="5895" activeTab="1" xr2:uid="{8FF49A41-D681-4C84-BD33-FF869755A9FC}"/>
   </bookViews>
@@ -508,12 +508,13 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>